<commit_message>
Casos pendientes al 95%
</commit_message>
<xml_diff>
--- a/Persona asignada.xlsx
+++ b/Persona asignada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intellego365-my.sharepoint.com/personal/luis_rincong_axity_com/Documents/Documentos/Proyectos/CORFICOLOMBIANA/Automatizaciones/ITSM/Corrección/Proyecto/Automatizacion_ITSM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_AD4D2F04E46CFB4ACB3E20F4F594E242693EDF24" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F11C52FB-B2EB-4575-9851-20B9750CD59A}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_AD4D2F04E46CFB4ACB3E20F4F594E242693EDF24" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF1B3759-D93A-4940-B6F9-F189722D87D0}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Persona asignada</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Erika Carolina Zamudio</t>
   </si>
   <si>
-    <t>James Andres Urquiza</t>
-  </si>
-  <si>
     <t>Dennis Carolina Holguin</t>
   </si>
   <si>
@@ -48,7 +45,10 @@
     <t>correo</t>
   </si>
   <si>
-    <t>David.Dorado@axity.com</t>
+    <t>Luis.RinconG@axity.com</t>
+  </si>
+  <si>
+    <t>Luis Carlos Rincon Gordo</t>
   </si>
 </sst>
 </file>
@@ -386,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -398,45 +398,55 @@
     <col min="2" max="2" width="21.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D7" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{A336FC8C-0E98-4351-87D6-252EA1D01C59}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{2039C93D-A024-492B-8C6B-0235DCD51595}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>